<commit_message>
added new player table, added csv import of players
</commit_message>
<xml_diff>
--- a/dev/startgroup.xlsx
+++ b/dev/startgroup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\mcs\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2A0629D-45F4-4348-B45D-43EA6730C1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45353648-2A27-4FDF-8209-F98833215B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{42B7B090-E56F-4169-A643-9840ECE72ABD}"/>
   </bookViews>
@@ -764,7 +764,7 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>